<commit_message>
chore: aggiorna workspace e file di test
</commit_message>
<xml_diff>
--- a/tmp_test_table_ddl/ddl.xlsx
+++ b/tmp_test_table_ddl/ddl.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,11 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
+          <t>ObjectType</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
           <t>DDL</t>
         </is>
       </c>
@@ -482,6 +487,11 @@
         </is>
       </c>
       <c r="E2" t="inlineStr">
+        <is>
+          <t>Sconosciuto</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
         <is>
           <t>CREATE TABLE [dbo].[t1] ( [id] int NOT NULL )</t>
         </is>

</xml_diff>